<commit_message>
Before switching pcts to raw numbers
</commit_message>
<xml_diff>
--- a/data-raw/Disability by Elementary.xlsx
+++ b/data-raw/Disability by Elementary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Shared\ADMN\WPSHARE\CYF\Early Learning Washington County\Data and Research\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidkeyes/Documents/Work/R for the Rest of Us/clients/PRE/washcomap/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C12C3A46-4436-4ADD-9FF0-17DB934CFB95}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1A1CF7D-9E06-BE45-9367-A1D571ED9403}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="820" yWindow="460" windowWidth="27980" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$83</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
@@ -208,9 +208,6 @@
     <t>Free Orchards Elementary School</t>
   </si>
   <si>
-    <t>Groner K-8</t>
-  </si>
-  <si>
     <t>Imlay Elementary School</t>
   </si>
   <si>
@@ -323,12 +320,15 @@
   </si>
   <si>
     <t>Median = 67</t>
+  </si>
+  <si>
+    <t>Groner Elementary School</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1197,26 +1197,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="B72" sqref="B72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.42578125" customWidth="1"/>
-    <col min="2" max="2" width="44.140625" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" customWidth="1"/>
-    <col min="4" max="4" width="5.42578125" customWidth="1"/>
-    <col min="5" max="5" width="6.5703125" customWidth="1"/>
-    <col min="6" max="6" width="5.7109375" customWidth="1"/>
-    <col min="7" max="7" width="23.140625" customWidth="1"/>
-    <col min="10" max="10" width="12.85546875" customWidth="1"/>
+    <col min="1" max="1" width="26.5" customWidth="1"/>
+    <col min="2" max="2" width="44.1640625" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" customWidth="1"/>
+    <col min="4" max="4" width="5.5" customWidth="1"/>
+    <col min="5" max="5" width="6.5" customWidth="1"/>
+    <col min="6" max="6" width="5.6640625" customWidth="1"/>
+    <col min="7" max="7" width="23.1640625" customWidth="1"/>
+    <col min="10" max="10" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1233,13 +1233,13 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G1" t="s">
         <v>97</v>
       </c>
-      <c r="G1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
         <v>8</v>
       </c>
@@ -1263,10 +1263,10 @@
         <v>1.9328358208955223</v>
       </c>
       <c r="J2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
         <v>8</v>
       </c>
@@ -1290,7 +1290,7 @@
         <v>1.8234328358208955</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
         <v>8</v>
       </c>
@@ -1314,7 +1314,7 @@
         <v>1.7677611940298508</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="15" t="s">
         <v>8</v>
       </c>
@@ -1338,12 +1338,12 @@
         <v>1.6771641791044776</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="s">
         <v>55</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C6" s="15" t="s">
         <v>49</v>
@@ -1362,7 +1362,7 @@
         <v>1.6713432835820896</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
         <v>8</v>
       </c>
@@ -1386,12 +1386,12 @@
         <v>1.556865671641791</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="15" t="s">
         <v>55</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C8" s="15" t="s">
         <v>49</v>
@@ -1410,7 +1410,7 @@
         <v>1.4982089552238804</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>8</v>
       </c>
@@ -1434,7 +1434,7 @@
         <v>1.4250746268656718</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
         <v>8</v>
       </c>
@@ -1458,12 +1458,12 @@
         <v>1.4198507462686567</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>55</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C11" s="12" t="s">
         <v>49</v>
@@ -1482,7 +1482,7 @@
         <v>1.4056716417910449</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="12" t="s">
         <v>8</v>
       </c>
@@ -1506,12 +1506,12 @@
         <v>1.3947761194029851</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C13" s="12" t="s">
         <v>7</v>
@@ -1530,12 +1530,12 @@
         <v>1.3922388059701494</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="12" t="s">
         <v>55</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C14" s="12" t="s">
         <v>49</v>
@@ -1554,7 +1554,7 @@
         <v>1.3823880597014926</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="12" t="s">
         <v>44</v>
       </c>
@@ -1578,7 +1578,7 @@
         <v>1.3594029850746268</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>8</v>
       </c>
@@ -1602,12 +1602,12 @@
         <v>1.3444776119402986</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>55</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C17" s="12" t="s">
         <v>49</v>
@@ -1626,12 +1626,12 @@
         <v>1.3331343283582091</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>55</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C18" s="12" t="s">
         <v>49</v>
@@ -1650,7 +1650,7 @@
         <v>1.2591044776119402</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>8</v>
       </c>
@@ -1674,7 +1674,7 @@
         <v>1.2559701492537314</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="12" t="s">
         <v>44</v>
       </c>
@@ -1698,12 +1698,12 @@
         <v>1.2508955223880598</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="9" t="s">
         <v>55</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>49</v>
@@ -1722,7 +1722,7 @@
         <v>1.2417910447761193</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="9" t="s">
         <v>8</v>
       </c>
@@ -1746,12 +1746,12 @@
         <v>1.2277611940298505</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="9" t="s">
         <v>55</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C23" s="9" t="s">
         <v>49</v>
@@ -1770,7 +1770,7 @@
         <v>1.2229850746268658</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="9" t="s">
         <v>55</v>
       </c>
@@ -1794,12 +1794,12 @@
         <v>1.2161194029850746</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="9" t="s">
         <v>55</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>49</v>
@@ -1818,7 +1818,7 @@
         <v>1.2067164179104477</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="9" t="s">
         <v>8</v>
       </c>
@@ -1842,7 +1842,7 @@
         <v>1.1888059701492537</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="9" t="s">
         <v>8</v>
       </c>
@@ -1866,12 +1866,12 @@
         <v>1.1837313432835821</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="9" t="s">
         <v>55</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C28" s="9" t="s">
         <v>49</v>
@@ -1890,7 +1890,7 @@
         <v>1.1691044776119404</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="9" t="s">
         <v>5</v>
       </c>
@@ -1914,12 +1914,12 @@
         <v>1.1677611940298507</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="9" t="s">
         <v>55</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C30" s="9" t="s">
         <v>49</v>
@@ -1938,7 +1938,7 @@
         <v>1.1346268656716418</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
         <v>8</v>
       </c>
@@ -1962,7 +1962,7 @@
         <v>1.1149253731343285</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
         <v>55</v>
       </c>
@@ -1986,7 +1986,7 @@
         <v>1.1062686567164179</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
         <v>8</v>
       </c>
@@ -2010,7 +2010,7 @@
         <v>1.0962686567164179</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
         <v>55</v>
       </c>
@@ -2034,7 +2034,7 @@
         <v>1.0868656716417913</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="s">
         <v>8</v>
       </c>
@@ -2058,7 +2058,7 @@
         <v>1.0688059701492538</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="6" t="s">
         <v>44</v>
       </c>
@@ -2082,12 +2082,12 @@
         <v>1.0682089552238807</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="6" t="s">
         <v>55</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C37" s="6" t="s">
         <v>49</v>
@@ -2106,12 +2106,12 @@
         <v>1.0510447761194031</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C38" s="6" t="s">
         <v>7</v>
@@ -2130,7 +2130,7 @@
         <v>1.0392537313432835</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="6" t="s">
         <v>55</v>
       </c>
@@ -2154,12 +2154,12 @@
         <v>1.0180597014925372</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="6" t="s">
         <v>55</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C40" s="6" t="s">
         <v>49</v>
@@ -2178,7 +2178,7 @@
         <v>1.0119402985074626</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="6" t="s">
         <v>8</v>
       </c>
@@ -2202,7 +2202,7 @@
         <v>1.0052238805970148</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="6" t="s">
         <v>8</v>
       </c>
@@ -2226,12 +2226,12 @@
         <v>0.99880597014925376</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>7</v>
@@ -2250,7 +2250,7 @@
         <v>0.9940298507462686</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>8</v>
       </c>
@@ -2274,7 +2274,7 @@
         <v>0.99134328358208956</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>8</v>
       </c>
@@ -2298,7 +2298,7 @@
         <v>0.98970149253731343</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>8</v>
       </c>
@@ -2322,7 +2322,7 @@
         <v>0.9850746268656716</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
         <v>8</v>
       </c>
@@ -2346,12 +2346,12 @@
         <v>0.98059701492537321</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C48" s="3" t="s">
         <v>7</v>
@@ -2370,12 +2370,12 @@
         <v>0.97194029850746277</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
         <v>55</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>49</v>
@@ -2394,12 +2394,12 @@
         <v>0.9695522388059703</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C50" s="3" t="s">
         <v>7</v>
@@ -2418,12 +2418,12 @@
         <v>0.96537313432835836</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B51" s="3" t="s">
         <v>81</v>
-      </c>
-      <c r="B51" s="3" t="s">
-        <v>82</v>
       </c>
       <c r="C51" s="3" t="s">
         <v>7</v>
@@ -2442,7 +2442,7 @@
         <v>0.95552238805970147</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
         <v>8</v>
       </c>
@@ -2466,12 +2466,12 @@
         <v>0.9492537313432835</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C53" s="3" t="s">
         <v>7</v>
@@ -2490,12 +2490,12 @@
         <v>0.935223880597015</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
         <v>55</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C54" s="3" t="s">
         <v>49</v>
@@ -2514,7 +2514,7 @@
         <v>0.93313432835820886</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
         <v>8</v>
       </c>
@@ -2538,7 +2538,7 @@
         <v>0.93253731343283575</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
         <v>8</v>
       </c>
@@ -2562,7 +2562,7 @@
         <v>0.93014925373134327</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
         <v>8</v>
       </c>
@@ -2586,12 +2586,12 @@
         <v>0.91597014925373144</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C58" s="3" t="s">
         <v>7</v>
@@ -2610,7 +2610,7 @@
         <v>0.90626865671641788</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
         <v>53</v>
       </c>
@@ -2634,12 +2634,12 @@
         <v>0.88656716417910442</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
         <v>55</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C60" s="3" t="s">
         <v>49</v>
@@ -2658,12 +2658,12 @@
         <v>0.88179104477611947</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
         <v>55</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C61" s="3" t="s">
         <v>49</v>
@@ -2682,7 +2682,7 @@
         <v>0.84358208955223879</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
         <v>8</v>
       </c>
@@ -2706,12 +2706,12 @@
         <v>0.84179104477611943</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C63" s="3" t="s">
         <v>7</v>
@@ -2730,12 +2730,12 @@
         <v>0.81641791044776124</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C64" s="3" t="s">
         <v>7</v>
@@ -2754,7 +2754,7 @@
         <v>0.81268656716417909</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
         <v>8</v>
       </c>
@@ -2778,7 +2778,7 @@
         <v>0.80447761194029854</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
         <v>8</v>
       </c>
@@ -2802,12 +2802,12 @@
         <v>0.77970149253731347</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C67" s="3" t="s">
         <v>7</v>
@@ -2822,16 +2822,16 @@
         <v>52.199999999999996</v>
       </c>
       <c r="G67" s="5">
-        <f t="shared" ref="G67:G83" si="1">F67/67</f>
+        <f t="shared" ref="G67:G82" si="1">F67/67</f>
         <v>0.77910447761194024</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C68" s="3" t="s">
         <v>7</v>
@@ -2850,7 +2850,7 @@
         <v>0.77492537313432841</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
         <v>44</v>
       </c>
@@ -2874,12 +2874,12 @@
         <v>0.76895522388059712</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
         <v>55</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C70" s="3" t="s">
         <v>49</v>
@@ -2898,12 +2898,12 @@
         <v>0.75432835820895527</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
         <v>55</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>61</v>
+        <v>99</v>
       </c>
       <c r="C71" s="3" t="s">
         <v>10</v>
@@ -2922,12 +2922,12 @@
         <v>0.74149253731343279</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B72" s="3" t="s">
         <v>86</v>
-      </c>
-      <c r="B72" s="3" t="s">
-        <v>87</v>
       </c>
       <c r="C72" s="3" t="s">
         <v>7</v>
@@ -2946,12 +2946,12 @@
         <v>0.72805970149253729</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
         <v>55</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C73" s="3" t="s">
         <v>49</v>
@@ -2970,7 +2970,7 @@
         <v>0.70328358208955222</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
         <v>55</v>
       </c>
@@ -2994,12 +2994,12 @@
         <v>0.70074626865671641</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C75" s="3" t="s">
         <v>7</v>
@@ -3018,7 +3018,7 @@
         <v>0.68298507462686564</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
         <v>8</v>
       </c>
@@ -3042,7 +3042,7 @@
         <v>0.65507462686567175</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" s="3" t="s">
         <v>8</v>
       </c>
@@ -3066,7 +3066,7 @@
         <v>0.65462686567164174</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="s">
         <v>44</v>
       </c>
@@ -3090,7 +3090,7 @@
         <v>0.64477611940298496</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" s="3" t="s">
         <v>8</v>
       </c>
@@ -3114,7 +3114,7 @@
         <v>0.63432835820895528</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" s="3" t="s">
         <v>8</v>
       </c>
@@ -3138,7 +3138,7 @@
         <v>0.62776119402985064</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" s="3" t="s">
         <v>8</v>
       </c>
@@ -3162,7 +3162,7 @@
         <v>0.54447761194029842</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" s="3" t="s">
         <v>44</v>
       </c>
@@ -3186,13 +3186,13 @@
         <v>0.50641791044776119</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="F83" s="2"/>
       <c r="G83" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F83">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F83">
+  <autoFilter ref="A1:F83" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <sortState ref="A2:F83">
       <sortCondition descending="1" ref="F1:F83"/>
     </sortState>
   </autoFilter>

</xml_diff>